<commit_message>
🐛 fix: add sot models
</commit_message>
<xml_diff>
--- a/public/Icraft_Icore_Metrics_V3.30.0_subtotal.xlsx
+++ b/public/Icraft_Icore_Metrics_V3.30.0_subtotal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="21011" windowHeight="9275" activeTab="4"/>
+    <workbookView windowWidth="21011" windowHeight="9275" firstSheet="7" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="audio_EER" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1941" uniqueCount="229">
   <si>
     <t>Series</t>
   </si>
@@ -668,6 +668,33 @@
   </si>
   <si>
     <t>1*112*112*3</t>
+  </si>
+  <si>
+    <t>siamfc++</t>
+  </si>
+  <si>
+    <t>1*3*303*303</t>
+  </si>
+  <si>
+    <t>kld-pc, kld-pc</t>
+  </si>
+  <si>
+    <t>siamrpn++</t>
+  </si>
+  <si>
+    <t>1*3*255*255</t>
+  </si>
+  <si>
+    <t>kld-pt, kld-pt</t>
+  </si>
+  <si>
+    <t>ETTrack</t>
+  </si>
+  <si>
+    <t>1*3*288*288</t>
+  </si>
+  <si>
+    <t>kld-pc, null-pt</t>
   </si>
   <si>
     <t>PSNR</t>
@@ -735,7 +762,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,11 +782,17 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -1100,7 +1133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1246,6 +1279,64 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1346,31 +1437,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1379,119 +1467,122 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1559,10 +1650,31 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2195,7 +2307,7 @@
       <c r="M1" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="27" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2239,7 +2351,7 @@
       <c r="M2" s="20">
         <v>0.72</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="28">
         <v>0.778</v>
       </c>
     </row>
@@ -2283,7 +2395,7 @@
       <c r="M3" s="20">
         <v>0.735</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="28">
         <v>0.787</v>
       </c>
     </row>
@@ -2327,7 +2439,7 @@
       <c r="M4" s="20">
         <v>0.724</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="28">
         <v>0.779</v>
       </c>
     </row>
@@ -2409,10 +2521,10 @@
       <c r="M1" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="27" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2456,10 +2568,10 @@
       <c r="M2" s="20">
         <v>0.426321130596695</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="O2" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2503,10 +2615,10 @@
       <c r="M3" s="20">
         <v>0.4338</v>
       </c>
-      <c r="N3" s="24" t="s">
+      <c r="N3" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2550,10 +2662,10 @@
       <c r="M4" s="20">
         <v>0.3678</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="28">
         <v>0.6909</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="28">
         <v>0.4507</v>
       </c>
     </row>
@@ -2597,10 +2709,10 @@
       <c r="M5" s="20">
         <v>0.3725</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="28">
         <v>0.6918</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5" s="28">
         <v>0.4563</v>
       </c>
     </row>
@@ -2644,10 +2756,10 @@
       <c r="M6" s="20">
         <v>0.3682</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="28">
         <v>0.6905</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6" s="28">
         <v>0.4514</v>
       </c>
     </row>
@@ -2733,13 +2845,13 @@
       <c r="M1" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="P1" s="27" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2783,13 +2895,13 @@
       <c r="M2" s="20">
         <v>0.276</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="28">
         <v>0.48</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="28">
         <v>0.349</v>
       </c>
-      <c r="P2" s="24">
+      <c r="P2" s="28">
         <v>0.551</v>
       </c>
     </row>
@@ -2833,13 +2945,13 @@
       <c r="M3" s="20">
         <v>0.282</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="28">
         <v>0.488</v>
       </c>
-      <c r="O3" s="24">
+      <c r="O3" s="28">
         <v>0.367</v>
       </c>
-      <c r="P3" s="24">
+      <c r="P3" s="28">
         <v>0.559</v>
       </c>
     </row>
@@ -2883,13 +2995,13 @@
       <c r="M4" s="20">
         <v>0.277</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="28">
         <v>0.483</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="28">
         <v>0.36</v>
       </c>
-      <c r="P4" s="24">
+      <c r="P4" s="28">
         <v>0.553</v>
       </c>
     </row>
@@ -2933,13 +3045,13 @@
       <c r="M5" s="20">
         <v>0.327</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="28">
         <v>0.534</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5" s="28">
         <v>0.436</v>
       </c>
-      <c r="P5" s="24">
+      <c r="P5" s="28">
         <v>0.603</v>
       </c>
     </row>
@@ -2983,13 +3095,13 @@
       <c r="M6" s="20">
         <v>0.331</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="28">
         <v>0.538</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6" s="28">
         <v>0.441</v>
       </c>
-      <c r="P6" s="24">
+      <c r="P6" s="28">
         <v>0.608</v>
       </c>
     </row>
@@ -3033,13 +3145,13 @@
       <c r="M7" s="20">
         <v>0.327</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="28">
         <v>0.534</v>
       </c>
-      <c r="O7" s="24">
+      <c r="O7" s="28">
         <v>0.437</v>
       </c>
-      <c r="P7" s="24">
+      <c r="P7" s="28">
         <v>0.603</v>
       </c>
     </row>
@@ -3125,13 +3237,13 @@
       <c r="M1" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="P1" s="27" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3175,13 +3287,13 @@
       <c r="M2" s="20">
         <v>0.9623</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="28">
         <v>0.8612</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="28">
         <v>0.7924</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="P2" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3225,13 +3337,13 @@
       <c r="M3" s="20">
         <v>0.9626</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="28">
         <v>0.8629</v>
       </c>
-      <c r="O3" s="24">
+      <c r="O3" s="28">
         <v>0.794</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3275,13 +3387,13 @@
       <c r="M4" s="20">
         <v>0.9623</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="28">
         <v>0.8615</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="28">
         <v>0.7925</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3325,13 +3437,13 @@
       <c r="M5" s="20">
         <v>0.9579</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="28">
         <v>0.8315</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5" s="28">
         <v>0.7692</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="P5" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3375,13 +3487,13 @@
       <c r="M6" s="20">
         <v>0.9588</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="28">
         <v>0.8431</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6" s="28">
         <v>0.7761</v>
       </c>
-      <c r="P6" s="24" t="s">
+      <c r="P6" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3425,13 +3537,13 @@
       <c r="M7" s="20">
         <v>0.9578</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="28">
         <v>0.8315</v>
       </c>
-      <c r="O7" s="24">
+      <c r="O7" s="28">
         <v>0.769</v>
       </c>
-      <c r="P7" s="24" t="s">
+      <c r="P7" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3475,13 +3587,13 @@
       <c r="M8" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="N8" s="24" t="s">
+      <c r="N8" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="24">
+      <c r="O8" s="28">
         <v>0.6669</v>
       </c>
-      <c r="P8" s="24" t="s">
+      <c r="P8" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3525,13 +3637,13 @@
       <c r="M9" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="N9" s="24" t="s">
+      <c r="N9" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="24">
+      <c r="O9" s="28">
         <v>0.6687</v>
       </c>
-      <c r="P9" s="24" t="s">
+      <c r="P9" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3575,13 +3687,13 @@
       <c r="M10" s="20">
         <v>0.9403</v>
       </c>
-      <c r="N10" s="24">
+      <c r="N10" s="28">
         <v>0.8405</v>
       </c>
-      <c r="O10" s="24">
+      <c r="O10" s="28">
         <v>0.7655</v>
       </c>
-      <c r="P10" s="24">
+      <c r="P10" s="28">
         <v>0.891</v>
       </c>
     </row>
@@ -3625,13 +3737,13 @@
       <c r="M11" s="20">
         <v>0.9406</v>
       </c>
-      <c r="N11" s="24">
+      <c r="N11" s="28">
         <v>0.8546</v>
       </c>
-      <c r="O11" s="24">
+      <c r="O11" s="28">
         <v>0.7693</v>
       </c>
-      <c r="P11" s="24">
+      <c r="P11" s="28">
         <v>0.8924</v>
       </c>
     </row>
@@ -3675,13 +3787,13 @@
       <c r="M12" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="O12" s="24">
+      <c r="O12" s="28">
         <v>0.5148</v>
       </c>
-      <c r="P12" s="24" t="s">
+      <c r="P12" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3725,13 +3837,13 @@
       <c r="M13" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="N13" s="24" t="s">
+      <c r="N13" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="O13" s="24">
+      <c r="O13" s="28">
         <v>0.5387</v>
       </c>
-      <c r="P13" s="24" t="s">
+      <c r="P13" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3775,13 +3887,13 @@
       <c r="M14" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="N14" s="24" t="s">
+      <c r="N14" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="O14" s="24">
+      <c r="O14" s="28">
         <v>0.4218</v>
       </c>
-      <c r="P14" s="24" t="s">
+      <c r="P14" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3825,13 +3937,13 @@
       <c r="M15" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="N15" s="24" t="s">
+      <c r="N15" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="O15" s="24">
+      <c r="O15" s="28">
         <v>0.4355</v>
       </c>
-      <c r="P15" s="24" t="s">
+      <c r="P15" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3916,10 +4028,10 @@
       <c r="M1" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="27" t="s">
         <v>190</v>
       </c>
     </row>
@@ -3963,10 +4075,10 @@
       <c r="M2" s="22">
         <v>0.0479296192316117</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="28">
         <v>0.867217004299164</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="28">
         <v>0.790438809266047</v>
       </c>
     </row>
@@ -4010,10 +4122,10 @@
       <c r="M3" s="22">
         <v>0.0476</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="28">
         <v>0.8669</v>
       </c>
-      <c r="O3" s="24">
+      <c r="O3" s="28">
         <v>0.7919</v>
       </c>
     </row>
@@ -4057,10 +4169,10 @@
       <c r="M4" s="22">
         <v>0.0479</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="28">
         <v>0.8672</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="28">
         <v>0.7903</v>
       </c>
     </row>
@@ -4076,17 +4188,17 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet15"/>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
@@ -4144,10 +4256,10 @@
       <c r="M1" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="27" t="s">
         <v>196</v>
       </c>
     </row>
@@ -4191,10 +4303,10 @@
       <c r="M2" s="20">
         <v>0.5647</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="28">
         <v>0.5859</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="28">
         <v>0.6837</v>
       </c>
     </row>
@@ -4238,10 +4350,10 @@
       <c r="M3" s="20">
         <v>0.604</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="28">
         <v>0.6497</v>
       </c>
-      <c r="O3" s="24">
+      <c r="O3" s="28">
         <v>0.7153</v>
       </c>
     </row>
@@ -4285,10 +4397,10 @@
       <c r="M4" s="20">
         <v>0.0422</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="28">
         <v>0.1061</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="28">
         <v>0.0572</v>
       </c>
     </row>
@@ -4332,11 +4444,221 @@
       <c r="M5" s="20">
         <v>0.5806</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="28">
         <v>0.585</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5" s="28">
         <v>0.6697</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="12">
+        <v>-1</v>
+      </c>
+      <c r="I6" s="14">
+        <v>3.672</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="M6" s="30">
+        <v>0.5136</v>
+      </c>
+      <c r="N6" s="31">
+        <v>0.5218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="12">
+        <v>-1</v>
+      </c>
+      <c r="I7" s="14">
+        <v>5.9922</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="M7" s="30">
+        <v>0.5125</v>
+      </c>
+      <c r="N7" s="31">
+        <v>0.5194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12">
+        <v>-1</v>
+      </c>
+      <c r="I8" s="14">
+        <v>5.391</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="L8" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="M8" s="30">
+        <v>0.4473</v>
+      </c>
+      <c r="N8" s="31">
+        <v>0.4477</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="12">
+        <v>-1</v>
+      </c>
+      <c r="I9" s="14">
+        <v>12.008</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="L9" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="M9" s="30">
+        <v>0.4571</v>
+      </c>
+      <c r="N9" s="31">
+        <v>0.4573</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="12">
+        <v>-1</v>
+      </c>
+      <c r="I10" s="14">
+        <v>16.763</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="M10" s="30">
+        <v>0.2116</v>
+      </c>
+      <c r="N10" s="31">
+        <v>0.1278</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="12">
+        <v>-1</v>
+      </c>
+      <c r="I11" s="14">
+        <v>32.918</v>
+      </c>
+      <c r="K11" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="L11" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="M11" s="30">
+        <v>0.5694</v>
+      </c>
+      <c r="N11" s="31">
+        <v>0.5711</v>
       </c>
     </row>
   </sheetData>
@@ -4415,18 +4737,18 @@
         <v>11</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="8" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>16</v>
@@ -4453,7 +4775,7 @@
         <v>136</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="M2" s="22">
         <v>30.7665440717631</v>
@@ -4461,13 +4783,13 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="8" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>16</v>
@@ -4494,7 +4816,7 @@
         <v>136</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="M3" s="22">
         <v>31.8618</v>
@@ -4502,13 +4824,13 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="8" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>16</v>
@@ -4535,7 +4857,7 @@
         <v>18</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="M4" s="22">
         <v>17.6435</v>
@@ -4543,13 +4865,13 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="8" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>16</v>
@@ -4576,7 +4898,7 @@
         <v>18</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="M5" s="22">
         <v>17.7362</v>
@@ -4584,13 +4906,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="8" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>16</v>
@@ -4617,7 +4939,7 @@
         <v>38</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="M6" s="22">
         <v>43.62</v>
@@ -4625,13 +4947,13 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="8" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>16</v>
@@ -4658,7 +4980,7 @@
         <v>38</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="M7" s="22">
         <v>44.22</v>
@@ -4666,13 +4988,13 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>213</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>204</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>16</v>
@@ -4699,7 +5021,7 @@
         <v>136</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="M8" s="22">
         <v>30.8535</v>
@@ -4707,13 +5029,13 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>213</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>204</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>16</v>
@@ -4740,7 +5062,7 @@
         <v>136</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="M9" s="22">
         <v>31.8889</v>
@@ -4827,13 +5149,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="8" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>16</v>
@@ -4860,7 +5182,7 @@
         <v>136</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="M2" s="20">
         <v>0.9089</v>
@@ -4868,13 +5190,13 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="8" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>16</v>
@@ -4901,7 +5223,7 @@
         <v>136</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="M3" s="20">
         <v>0.9092</v>
@@ -4909,13 +5231,13 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="8" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>16</v>
@@ -4942,7 +5264,7 @@
         <v>136</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="M4" s="20">
         <v>0.87</v>
@@ -4950,13 +5272,13 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="8" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>16</v>
@@ -4983,7 +5305,7 @@
         <v>136</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="M5" s="20">
         <v>0.8362</v>
@@ -4991,13 +5313,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="8" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>16</v>
@@ -5024,7 +5346,7 @@
         <v>136</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="M6" s="20">
         <v>0.4184</v>
@@ -5032,13 +5354,13 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="8" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>16</v>
@@ -5065,7 +5387,7 @@
         <v>136</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="M7" s="20">
         <v>0.9455</v>
@@ -5558,7 +5880,7 @@
       <c r="M1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="27" t="s">
         <v>29</v>
       </c>
     </row>
@@ -5602,7 +5924,7 @@
       <c r="M2" s="20">
         <v>0.694084278768233</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5646,7 +5968,7 @@
       <c r="M3" s="20">
         <v>0.6864</v>
       </c>
-      <c r="N3" s="24" t="s">
+      <c r="N3" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5690,7 +6012,7 @@
       <c r="M4" s="20">
         <v>0.9455</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5734,7 +6056,7 @@
       <c r="M5" s="20">
         <v>0.9441</v>
       </c>
-      <c r="N5" s="24" t="s">
+      <c r="N5" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5778,7 +6100,7 @@
       <c r="M6" s="20">
         <v>0.9482</v>
       </c>
-      <c r="N6" s="24" t="s">
+      <c r="N6" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5822,7 +6144,7 @@
       <c r="M7" s="20">
         <v>0.6688</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="28">
         <v>0.8742</v>
       </c>
     </row>
@@ -5866,7 +6188,7 @@
       <c r="M8" s="20">
         <v>0.6798</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8" s="28">
         <v>0.8794</v>
       </c>
     </row>
@@ -5910,7 +6232,7 @@
       <c r="M9" s="20">
         <v>0.6672</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="28">
         <v>0.8744</v>
       </c>
     </row>
@@ -5954,7 +6276,7 @@
       <c r="M10" s="20">
         <v>0.7766</v>
       </c>
-      <c r="N10" s="24">
+      <c r="N10" s="28">
         <v>0.9344</v>
       </c>
     </row>
@@ -5998,7 +6320,7 @@
       <c r="M11" s="20">
         <v>0.812</v>
       </c>
-      <c r="N11" s="24">
+      <c r="N11" s="28">
         <v>0.9532</v>
       </c>
     </row>
@@ -6042,7 +6364,7 @@
       <c r="M12" s="20">
         <v>0.6936</v>
       </c>
-      <c r="N12" s="24">
+      <c r="N12" s="28">
         <v>0.889</v>
       </c>
     </row>
@@ -6086,7 +6408,7 @@
       <c r="M13" s="20">
         <v>0.7002</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13" s="28">
         <v>0.907</v>
       </c>
     </row>
@@ -6130,7 +6452,7 @@
       <c r="M14" s="20">
         <v>0.6922</v>
       </c>
-      <c r="N14" s="24">
+      <c r="N14" s="28">
         <v>0.8956</v>
       </c>
     </row>
@@ -6310,7 +6632,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="H46" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -6376,7 +6698,7 @@
       <c r="M1" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="27" t="s">
         <v>52</v>
       </c>
     </row>
@@ -6420,7 +6742,7 @@
       <c r="M2" s="20">
         <v>0.161</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="28">
         <v>0.328</v>
       </c>
     </row>
@@ -6464,7 +6786,7 @@
       <c r="M3" s="20">
         <v>0.35</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="28">
         <v>0.537</v>
       </c>
     </row>
@@ -6508,7 +6830,7 @@
       <c r="M4" s="20">
         <v>0.159</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="28">
         <v>0.327</v>
       </c>
     </row>
@@ -6552,7 +6874,7 @@
       <c r="M5" s="20">
         <v>0.384</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="28">
         <v>0.55</v>
       </c>
     </row>
@@ -6596,7 +6918,7 @@
       <c r="M6" s="20">
         <v>0.41</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="28">
         <v>0.585</v>
       </c>
     </row>
@@ -6640,7 +6962,7 @@
       <c r="M7" s="20">
         <v>0.384</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="28">
         <v>0.55</v>
       </c>
     </row>
@@ -6684,7 +7006,7 @@
       <c r="M8" s="20">
         <v>0.35</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8" s="28">
         <v>0.551</v>
       </c>
     </row>
@@ -6728,7 +7050,7 @@
       <c r="M9" s="20">
         <v>0.37</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="28">
         <v>0.561</v>
       </c>
     </row>
@@ -6772,7 +7094,7 @@
       <c r="M10" s="20">
         <v>0.361</v>
       </c>
-      <c r="N10" s="24">
+      <c r="N10" s="28">
         <v>0.555</v>
       </c>
     </row>
@@ -6816,7 +7138,7 @@
       <c r="M11" s="20">
         <v>0.451</v>
       </c>
-      <c r="N11" s="24">
+      <c r="N11" s="28">
         <v>0.619</v>
       </c>
     </row>
@@ -6860,7 +7182,7 @@
       <c r="M12" s="20">
         <v>0.459</v>
       </c>
-      <c r="N12" s="24">
+      <c r="N12" s="28">
         <v>0.627</v>
       </c>
     </row>
@@ -6904,7 +7226,7 @@
       <c r="M13" s="20">
         <v>0.452</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13" s="28">
         <v>0.62</v>
       </c>
     </row>
@@ -6948,7 +7270,7 @@
       <c r="M14" s="20">
         <v>0.503</v>
       </c>
-      <c r="N14" s="24">
+      <c r="N14" s="28">
         <v>0.682</v>
       </c>
     </row>
@@ -6992,7 +7314,7 @@
       <c r="M15" s="20">
         <v>0.506</v>
       </c>
-      <c r="N15" s="24">
+      <c r="N15" s="28">
         <v>0.687</v>
       </c>
     </row>
@@ -7036,7 +7358,7 @@
       <c r="M16" s="20">
         <v>0.503</v>
       </c>
-      <c r="N16" s="24">
+      <c r="N16" s="28">
         <v>0.683</v>
       </c>
     </row>
@@ -7080,7 +7402,7 @@
       <c r="M17" s="20">
         <v>0.508</v>
       </c>
-      <c r="N17" s="24">
+      <c r="N17" s="28">
         <v>0.689</v>
       </c>
     </row>
@@ -7124,7 +7446,7 @@
       <c r="M18" s="20">
         <v>0.509</v>
       </c>
-      <c r="N18" s="24">
+      <c r="N18" s="28">
         <v>0.69</v>
       </c>
     </row>
@@ -7168,7 +7490,7 @@
       <c r="M19" s="20">
         <v>0.509</v>
       </c>
-      <c r="N19" s="24">
+      <c r="N19" s="28">
         <v>0.689</v>
       </c>
     </row>
@@ -7212,7 +7534,7 @@
       <c r="M20" s="20">
         <v>0.486</v>
       </c>
-      <c r="N20" s="24">
+      <c r="N20" s="28">
         <v>0.663</v>
       </c>
     </row>
@@ -7256,7 +7578,7 @@
       <c r="M21" s="20">
         <v>0.49</v>
       </c>
-      <c r="N21" s="24">
+      <c r="N21" s="28">
         <v>0.668</v>
       </c>
     </row>
@@ -7300,7 +7622,7 @@
       <c r="M22" s="20">
         <v>0.487</v>
       </c>
-      <c r="N22" s="24">
+      <c r="N22" s="28">
         <v>0.663</v>
       </c>
     </row>
@@ -7344,7 +7666,7 @@
       <c r="M23" s="20">
         <v>0.363</v>
       </c>
-      <c r="N23" s="24">
+      <c r="N23" s="28">
         <v>0.519</v>
       </c>
     </row>
@@ -7388,7 +7710,7 @@
       <c r="M24" s="20">
         <v>0.373</v>
       </c>
-      <c r="N24" s="24">
+      <c r="N24" s="28">
         <v>0.53</v>
       </c>
     </row>
@@ -7432,7 +7754,7 @@
       <c r="M25" s="20">
         <v>0.364</v>
       </c>
-      <c r="N25" s="24">
+      <c r="N25" s="28">
         <v>0.52</v>
       </c>
     </row>
@@ -7476,7 +7798,7 @@
       <c r="M26" s="20">
         <v>0.447</v>
       </c>
-      <c r="N26" s="24">
+      <c r="N26" s="28">
         <v>0.622</v>
       </c>
     </row>
@@ -7520,7 +7842,7 @@
       <c r="M27" s="20">
         <v>0.45</v>
       </c>
-      <c r="N27" s="24">
+      <c r="N27" s="28">
         <v>0.627</v>
       </c>
     </row>
@@ -7564,7 +7886,7 @@
       <c r="M28" s="20">
         <v>0.447</v>
       </c>
-      <c r="N28" s="24">
+      <c r="N28" s="28">
         <v>0.622</v>
       </c>
     </row>
@@ -7608,7 +7930,7 @@
       <c r="M29" s="20">
         <v>0.521</v>
       </c>
-      <c r="N29" s="24">
+      <c r="N29" s="28">
         <v>0.698</v>
       </c>
     </row>
@@ -7652,7 +7974,7 @@
       <c r="M30" s="20">
         <v>0.525</v>
       </c>
-      <c r="N30" s="24">
+      <c r="N30" s="28">
         <v>0.702</v>
       </c>
     </row>
@@ -7696,7 +8018,7 @@
       <c r="M31" s="20">
         <v>0.523</v>
       </c>
-      <c r="N31" s="24">
+      <c r="N31" s="28">
         <v>0.699</v>
       </c>
     </row>
@@ -7740,7 +8062,7 @@
       <c r="M32" s="20">
         <v>0.518</v>
       </c>
-      <c r="N32" s="24">
+      <c r="N32" s="28">
         <v>0.686</v>
       </c>
     </row>
@@ -7784,7 +8106,7 @@
       <c r="M33" s="20">
         <v>0.52</v>
       </c>
-      <c r="N33" s="24">
+      <c r="N33" s="28">
         <v>0.69</v>
       </c>
     </row>
@@ -7828,7 +8150,7 @@
       <c r="M34" s="20">
         <v>0.518</v>
       </c>
-      <c r="N34" s="24">
+      <c r="N34" s="28">
         <v>0.687</v>
       </c>
     </row>
@@ -7872,7 +8194,7 @@
       <c r="M35" s="20">
         <v>0.503</v>
       </c>
-      <c r="N35" s="24">
+      <c r="N35" s="28">
         <v>0.675</v>
       </c>
     </row>
@@ -7916,7 +8238,7 @@
       <c r="M36" s="20">
         <v>0.509</v>
       </c>
-      <c r="N36" s="24">
+      <c r="N36" s="28">
         <v>0.68</v>
       </c>
     </row>
@@ -7960,7 +8282,7 @@
       <c r="M37" s="20">
         <v>0.504</v>
       </c>
-      <c r="N37" s="24">
+      <c r="N37" s="28">
         <v>0.675</v>
       </c>
     </row>
@@ -8004,7 +8326,7 @@
       <c r="M38" s="20">
         <v>0.366</v>
       </c>
-      <c r="N38" s="24">
+      <c r="N38" s="28">
         <v>0.51</v>
       </c>
     </row>
@@ -8048,7 +8370,7 @@
       <c r="M39" s="20">
         <v>0.373</v>
       </c>
-      <c r="N39" s="24">
+      <c r="N39" s="28">
         <v>0.517</v>
       </c>
     </row>
@@ -8092,7 +8414,7 @@
       <c r="M40" s="20">
         <v>0.366</v>
       </c>
-      <c r="N40" s="24">
+      <c r="N40" s="28">
         <v>0.51</v>
       </c>
     </row>
@@ -8136,7 +8458,7 @@
       <c r="M41" s="20">
         <v>0.452</v>
       </c>
-      <c r="N41" s="24">
+      <c r="N41" s="28">
         <v>0.616</v>
       </c>
     </row>
@@ -8180,7 +8502,7 @@
       <c r="M42" s="20">
         <v>0.458</v>
       </c>
-      <c r="N42" s="24">
+      <c r="N42" s="28">
         <v>0.623</v>
       </c>
     </row>
@@ -8224,7 +8546,7 @@
       <c r="M43" s="20">
         <v>0.452</v>
       </c>
-      <c r="N43" s="24">
+      <c r="N43" s="28">
         <v>0.617</v>
       </c>
     </row>
@@ -8268,7 +8590,7 @@
       <c r="M44" s="20">
         <v>0.532</v>
       </c>
-      <c r="N44" s="24">
+      <c r="N44" s="28">
         <v>0.703</v>
       </c>
     </row>
@@ -8312,7 +8634,7 @@
       <c r="M45" s="20">
         <v>0.535</v>
       </c>
-      <c r="N45" s="24">
+      <c r="N45" s="28">
         <v>0.705</v>
       </c>
     </row>
@@ -8356,7 +8678,7 @@
       <c r="M46" s="20">
         <v>0.533</v>
       </c>
-      <c r="N46" s="24">
+      <c r="N46" s="28">
         <v>0.703</v>
       </c>
     </row>
@@ -8400,7 +8722,7 @@
       <c r="M47" s="20">
         <v>0.454</v>
       </c>
-      <c r="N47" s="24">
+      <c r="N47" s="28">
         <v>0.663</v>
       </c>
     </row>
@@ -8444,7 +8766,7 @@
       <c r="M48" s="20">
         <v>0.479</v>
       </c>
-      <c r="N48" s="24">
+      <c r="N48" s="28">
         <v>0.668</v>
       </c>
     </row>
@@ -8488,7 +8810,7 @@
       <c r="M49" s="20">
         <v>0.475</v>
       </c>
-      <c r="N49" s="24">
+      <c r="N49" s="28">
         <v>0.665</v>
       </c>
     </row>
@@ -8532,7 +8854,7 @@
       <c r="M50" s="20">
         <v>0.422</v>
       </c>
-      <c r="N50" s="24">
+      <c r="N50" s="28">
         <v>0.632</v>
       </c>
     </row>
@@ -8576,7 +8898,7 @@
       <c r="M51" s="20">
         <v>0.441</v>
       </c>
-      <c r="N51" s="24">
+      <c r="N51" s="28">
         <v>0.637</v>
       </c>
     </row>
@@ -8620,7 +8942,7 @@
       <c r="M52" s="20">
         <v>0.434</v>
       </c>
-      <c r="N52" s="24">
+      <c r="N52" s="28">
         <v>0.634</v>
       </c>
     </row>
@@ -8664,7 +8986,7 @@
       <c r="M53" s="20">
         <v>0.258</v>
       </c>
-      <c r="N53" s="24">
+      <c r="N53" s="28">
         <v>0.443</v>
       </c>
     </row>
@@ -8708,7 +9030,7 @@
       <c r="M54" s="20">
         <v>0.274</v>
       </c>
-      <c r="N54" s="24">
+      <c r="N54" s="28">
         <v>0.453</v>
       </c>
     </row>
@@ -8752,7 +9074,7 @@
       <c r="M55" s="20">
         <v>0.266</v>
       </c>
-      <c r="N55" s="24">
+      <c r="N55" s="28">
         <v>0.446</v>
       </c>
     </row>
@@ -8796,7 +9118,7 @@
       <c r="M56" s="20">
         <v>0.35</v>
       </c>
-      <c r="N56" s="24">
+      <c r="N56" s="28">
         <v>0.556</v>
       </c>
     </row>
@@ -8840,7 +9162,7 @@
       <c r="M57" s="20">
         <v>0.37</v>
       </c>
-      <c r="N57" s="24">
+      <c r="N57" s="28">
         <v>0.565</v>
       </c>
     </row>
@@ -8884,7 +9206,7 @@
       <c r="M58" s="20">
         <v>0.361</v>
       </c>
-      <c r="N58" s="24">
+      <c r="N58" s="28">
         <v>0.559</v>
       </c>
     </row>
@@ -8928,7 +9250,7 @@
       <c r="M59" s="20">
         <v>0.475</v>
       </c>
-      <c r="N59" s="24">
+      <c r="N59" s="28">
         <v>0.683</v>
       </c>
     </row>
@@ -8972,7 +9294,7 @@
       <c r="M60" s="20">
         <v>0.497</v>
       </c>
-      <c r="N60" s="24">
+      <c r="N60" s="28">
         <v>0.686</v>
       </c>
     </row>
@@ -9016,7 +9338,7 @@
       <c r="M61" s="20">
         <v>0.493</v>
       </c>
-      <c r="N61" s="24">
+      <c r="N61" s="28">
         <v>0.686</v>
       </c>
     </row>
@@ -9060,7 +9382,7 @@
       <c r="M62" s="20">
         <v>0.3935</v>
       </c>
-      <c r="N62" s="24">
+      <c r="N62" s="28">
         <v>0.6701</v>
       </c>
     </row>
@@ -9104,7 +9426,7 @@
       <c r="M63" s="20">
         <v>0.4073</v>
       </c>
-      <c r="N63" s="24">
+      <c r="N63" s="28">
         <v>0.6771</v>
       </c>
     </row>
@@ -9148,7 +9470,7 @@
       <c r="M64" s="20">
         <v>0.4036</v>
       </c>
-      <c r="N64" s="24">
+      <c r="N64" s="28">
         <v>0.6737</v>
       </c>
     </row>
@@ -9272,7 +9594,7 @@
       <c r="M67" s="20">
         <v>0.41</v>
       </c>
-      <c r="N67" s="24">
+      <c r="N67" s="28">
         <v>0.62</v>
       </c>
     </row>
@@ -9316,7 +9638,7 @@
       <c r="M68" s="20">
         <v>0.434</v>
       </c>
-      <c r="N68" s="24">
+      <c r="N68" s="28">
         <v>0.628</v>
       </c>
     </row>
@@ -9360,7 +9682,7 @@
       <c r="M69" s="20">
         <v>0.429</v>
       </c>
-      <c r="N69" s="24">
+      <c r="N69" s="28">
         <v>0.624</v>
       </c>
     </row>
@@ -9404,7 +9726,7 @@
       <c r="M70" s="20">
         <v>0.409</v>
       </c>
-      <c r="N70" s="24">
+      <c r="N70" s="28">
         <v>0.585</v>
       </c>
     </row>
@@ -9448,7 +9770,7 @@
       <c r="M71" s="20">
         <v>0.424</v>
       </c>
-      <c r="N71" s="24">
+      <c r="N71" s="28">
         <v>0.592</v>
       </c>
     </row>
@@ -9492,7 +9814,7 @@
       <c r="M72" s="20">
         <v>0.415</v>
       </c>
-      <c r="N72" s="24">
+      <c r="N72" s="28">
         <v>0.587</v>
       </c>
     </row>
@@ -9536,7 +9858,7 @@
       <c r="M73" s="20">
         <v>0.462</v>
       </c>
-      <c r="N73" s="24">
+      <c r="N73" s="28">
         <v>0.684</v>
       </c>
     </row>
@@ -9580,7 +9902,7 @@
       <c r="M74" s="20">
         <v>0.509</v>
       </c>
-      <c r="N74" s="24">
+      <c r="N74" s="28">
         <v>0.692</v>
       </c>
     </row>
@@ -9624,7 +9946,7 @@
       <c r="M75" s="20">
         <v>0.495</v>
       </c>
-      <c r="N75" s="24">
+      <c r="N75" s="28">
         <v>0.69</v>
       </c>
     </row>
@@ -9668,7 +9990,7 @@
       <c r="M76" s="20">
         <v>0.338</v>
       </c>
-      <c r="N76" s="24">
+      <c r="N76" s="28">
         <v>0.535</v>
       </c>
     </row>
@@ -9712,7 +10034,7 @@
       <c r="M77" s="20">
         <v>0.367</v>
       </c>
-      <c r="N77" s="24">
+      <c r="N77" s="28">
         <v>0.545</v>
       </c>
     </row>
@@ -9756,7 +10078,7 @@
       <c r="M78" s="20">
         <v>0.363</v>
       </c>
-      <c r="N78" s="24">
+      <c r="N78" s="28">
         <v>0.543</v>
       </c>
     </row>
@@ -9800,7 +10122,7 @@
       <c r="M79" s="20">
         <v>0.49</v>
       </c>
-      <c r="N79" s="24">
+      <c r="N79" s="28">
         <v>0.703</v>
       </c>
     </row>
@@ -9844,7 +10166,7 @@
       <c r="M80" s="20">
         <v>0.527</v>
       </c>
-      <c r="N80" s="24">
+      <c r="N80" s="28">
         <v>0.709</v>
       </c>
     </row>
@@ -9888,7 +10210,7 @@
       <c r="M81" s="20">
         <v>0.522</v>
       </c>
-      <c r="N81" s="24">
+      <c r="N81" s="28">
         <v>0.706</v>
       </c>
     </row>
@@ -9932,7 +10254,7 @@
       <c r="M82" s="20">
         <v>0.513</v>
       </c>
-      <c r="N82" s="24">
+      <c r="N82" s="28">
         <v>0.727</v>
       </c>
     </row>
@@ -9976,7 +10298,7 @@
       <c r="M83" s="20">
         <v>0.558</v>
       </c>
-      <c r="N83" s="24">
+      <c r="N83" s="28">
         <v>0.734</v>
       </c>
     </row>
@@ -10020,7 +10342,7 @@
       <c r="M84" s="20">
         <v>0.541</v>
       </c>
-      <c r="N84" s="24">
+      <c r="N84" s="28">
         <v>0.729</v>
       </c>
     </row>
@@ -10064,7 +10386,7 @@
       <c r="M85" s="20">
         <v>0.5</v>
       </c>
-      <c r="N85" s="24">
+      <c r="N85" s="28">
         <v>0.724</v>
       </c>
     </row>
@@ -10108,7 +10430,7 @@
       <c r="M86" s="20">
         <v>0.55</v>
       </c>
-      <c r="N86" s="24">
+      <c r="N86" s="28">
         <v>0.729</v>
       </c>
     </row>
@@ -10152,7 +10474,7 @@
       <c r="M87" s="20">
         <v>0.532</v>
       </c>
-      <c r="N87" s="24">
+      <c r="N87" s="28">
         <v>0.727</v>
       </c>
     </row>
@@ -10196,7 +10518,7 @@
       <c r="M88" s="20">
         <v>0.519</v>
       </c>
-      <c r="N88" s="24">
+      <c r="N88" s="28">
         <v>0.734</v>
       </c>
     </row>
@@ -10240,7 +10562,7 @@
       <c r="M89" s="20">
         <v>0.562</v>
       </c>
-      <c r="N89" s="24">
+      <c r="N89" s="28">
         <v>0.739</v>
       </c>
     </row>
@@ -10284,7 +10606,7 @@
       <c r="M90" s="20">
         <v>0.551</v>
       </c>
-      <c r="N90" s="24">
+      <c r="N90" s="28">
         <v>0.736</v>
       </c>
     </row>
@@ -10328,7 +10650,7 @@
       <c r="M91" s="20">
         <v>0.492</v>
       </c>
-      <c r="N91" s="24">
+      <c r="N91" s="28">
         <v>0.711</v>
       </c>
     </row>
@@ -10372,7 +10694,7 @@
       <c r="M92" s="20">
         <v>0.538</v>
       </c>
-      <c r="N92" s="24">
+      <c r="N92" s="28">
         <v>0.715</v>
       </c>
     </row>
@@ -10416,7 +10738,7 @@
       <c r="M93" s="20">
         <v>0.521</v>
       </c>
-      <c r="N93" s="24">
+      <c r="N93" s="28">
         <v>0.715</v>
       </c>
     </row>
@@ -10460,7 +10782,7 @@
       <c r="M94" s="20">
         <v>0.52</v>
       </c>
-      <c r="N94" s="24">
+      <c r="N94" s="28">
         <v>0.691</v>
       </c>
     </row>
@@ -10504,7 +10826,7 @@
       <c r="M95" s="20">
         <v>0.524</v>
       </c>
-      <c r="N95" s="24">
+      <c r="N95" s="28">
         <v>0.695</v>
       </c>
     </row>
@@ -10548,7 +10870,7 @@
       <c r="M96" s="20">
         <v>0.521</v>
       </c>
-      <c r="N96" s="24">
+      <c r="N96" s="28">
         <v>0.691</v>
       </c>
     </row>
@@ -10592,7 +10914,7 @@
       <c r="M97" s="20">
         <v>0.496</v>
       </c>
-      <c r="N97" s="24">
+      <c r="N97" s="28">
         <v>0.669</v>
       </c>
     </row>
@@ -10636,7 +10958,7 @@
       <c r="M98" s="20">
         <v>0.499</v>
       </c>
-      <c r="N98" s="24">
+      <c r="N98" s="28">
         <v>0.67</v>
       </c>
     </row>
@@ -10680,7 +11002,7 @@
       <c r="M99" s="20">
         <v>0.497</v>
       </c>
-      <c r="N99" s="24">
+      <c r="N99" s="28">
         <v>0.669</v>
       </c>
     </row>
@@ -10724,7 +11046,7 @@
       <c r="M100" s="20">
         <v>0.362</v>
       </c>
-      <c r="N100" s="24">
+      <c r="N100" s="28">
         <v>0.518</v>
       </c>
     </row>
@@ -10768,7 +11090,7 @@
       <c r="M101" s="20">
         <v>0.368</v>
       </c>
-      <c r="N101" s="24">
+      <c r="N101" s="28">
         <v>0.524</v>
       </c>
     </row>
@@ -10812,7 +11134,7 @@
       <c r="M102" s="20">
         <v>0.363</v>
       </c>
-      <c r="N102" s="24">
+      <c r="N102" s="28">
         <v>0.518</v>
       </c>
     </row>
@@ -10856,7 +11178,7 @@
       <c r="M103" s="20">
         <v>0.439</v>
       </c>
-      <c r="N103" s="24">
+      <c r="N103" s="28">
         <v>0.61</v>
       </c>
     </row>
@@ -10900,7 +11222,7 @@
       <c r="M104" s="20">
         <v>0.444</v>
       </c>
-      <c r="N104" s="24">
+      <c r="N104" s="28">
         <v>0.614</v>
       </c>
     </row>
@@ -10944,7 +11266,7 @@
       <c r="M105" s="20">
         <v>0.44</v>
       </c>
-      <c r="N105" s="24">
+      <c r="N105" s="28">
         <v>0.61</v>
       </c>
     </row>
@@ -10988,7 +11310,7 @@
       <c r="M106" s="20">
         <v>0.532</v>
       </c>
-      <c r="N106" s="24">
+      <c r="N106" s="28">
         <v>0.705</v>
       </c>
     </row>
@@ -11032,7 +11354,7 @@
       <c r="M107" s="20">
         <v>0.535</v>
       </c>
-      <c r="N107" s="24">
+      <c r="N107" s="28">
         <v>0.707</v>
       </c>
     </row>
@@ -11076,7 +11398,7 @@
       <c r="M108" s="20">
         <v>0.534</v>
       </c>
-      <c r="N108" s="24">
+      <c r="N108" s="28">
         <v>0.705</v>
       </c>
     </row>
@@ -11120,7 +11442,7 @@
       <c r="M109" s="20">
         <v>0.523</v>
       </c>
-      <c r="N109" s="24">
+      <c r="N109" s="28">
         <v>0.694</v>
       </c>
     </row>
@@ -11164,7 +11486,7 @@
       <c r="M110" s="20">
         <v>0.526</v>
       </c>
-      <c r="N110" s="24">
+      <c r="N110" s="28">
         <v>0.698</v>
       </c>
     </row>
@@ -11208,7 +11530,7 @@
       <c r="M111" s="20">
         <v>0.523</v>
       </c>
-      <c r="N111" s="24">
+      <c r="N111" s="28">
         <v>0.694</v>
       </c>
     </row>
@@ -11252,7 +11574,7 @@
       <c r="M112" s="20">
         <v>0.505</v>
       </c>
-      <c r="N112" s="24">
+      <c r="N112" s="28">
         <v>0.672</v>
       </c>
     </row>
@@ -11296,7 +11618,7 @@
       <c r="M113" s="20">
         <v>0.509</v>
       </c>
-      <c r="N113" s="24">
+      <c r="N113" s="28">
         <v>0.675</v>
       </c>
     </row>
@@ -11340,7 +11662,7 @@
       <c r="M114" s="20">
         <v>0.505</v>
       </c>
-      <c r="N114" s="24">
+      <c r="N114" s="28">
         <v>0.672</v>
       </c>
     </row>
@@ -11384,7 +11706,7 @@
       <c r="M115" s="20">
         <v>0.408</v>
       </c>
-      <c r="N115" s="24">
+      <c r="N115" s="28">
         <v>0.571</v>
       </c>
     </row>
@@ -11428,7 +11750,7 @@
       <c r="M116" s="20">
         <v>0.461</v>
       </c>
-      <c r="N116" s="24">
+      <c r="N116" s="28">
         <v>0.625</v>
       </c>
     </row>
@@ -11472,7 +11794,7 @@
       <c r="M117" s="20">
         <v>0.427</v>
       </c>
-      <c r="N117" s="24">
+      <c r="N117" s="28">
         <v>0.591</v>
       </c>
     </row>
@@ -11516,7 +11838,7 @@
       <c r="M118" s="20">
         <v>0.346</v>
       </c>
-      <c r="N118" s="24">
+      <c r="N118" s="28">
         <v>0.49</v>
       </c>
     </row>
@@ -11560,7 +11882,7 @@
       <c r="M119" s="20">
         <v>0.37</v>
       </c>
-      <c r="N119" s="24">
+      <c r="N119" s="28">
         <v>0.521</v>
       </c>
     </row>
@@ -11604,7 +11926,7 @@
       <c r="M120" s="20">
         <v>0.351</v>
       </c>
-      <c r="N120" s="24">
+      <c r="N120" s="28">
         <v>0.496</v>
       </c>
     </row>
@@ -11648,7 +11970,7 @@
       <c r="M121" s="20">
         <v>0.461</v>
       </c>
-      <c r="N121" s="24">
+      <c r="N121" s="28">
         <v>0.673</v>
       </c>
     </row>
@@ -11692,7 +12014,7 @@
       <c r="M122" s="20">
         <v>0.478</v>
       </c>
-      <c r="N122" s="24">
+      <c r="N122" s="28">
         <v>0.682</v>
       </c>
     </row>
@@ -11736,7 +12058,7 @@
       <c r="M123" s="20">
         <v>0.461</v>
       </c>
-      <c r="N123" s="24">
+      <c r="N123" s="28">
         <v>0.673</v>
       </c>
     </row>
@@ -11780,7 +12102,7 @@
       <c r="M124" s="20">
         <v>0.445</v>
       </c>
-      <c r="N124" s="24">
+      <c r="N124" s="28">
         <v>0.643</v>
       </c>
     </row>
@@ -11824,7 +12146,7 @@
       <c r="M125" s="20">
         <v>0.463</v>
       </c>
-      <c r="N125" s="24">
+      <c r="N125" s="28">
         <v>0.655</v>
       </c>
     </row>
@@ -11868,7 +12190,7 @@
       <c r="M126" s="20">
         <v>0.444</v>
       </c>
-      <c r="N126" s="24">
+      <c r="N126" s="28">
         <v>0.643</v>
       </c>
     </row>
@@ -11912,7 +12234,7 @@
       <c r="M127" s="20">
         <v>0.388</v>
       </c>
-      <c r="N127" s="24">
+      <c r="N127" s="28">
         <v>0.582</v>
       </c>
     </row>
@@ -11956,7 +12278,7 @@
       <c r="M128" s="20">
         <v>0.405</v>
       </c>
-      <c r="N128" s="24">
+      <c r="N128" s="28">
         <v>0.592</v>
       </c>
     </row>
@@ -12000,7 +12322,7 @@
       <c r="M129" s="20">
         <v>0.388</v>
       </c>
-      <c r="N129" s="24">
+      <c r="N129" s="28">
         <v>0.582</v>
       </c>
     </row>
@@ -12044,7 +12366,7 @@
       <c r="M130" s="20">
         <v>0.31</v>
       </c>
-      <c r="N130" s="24">
+      <c r="N130" s="28">
         <v>0.489</v>
       </c>
     </row>
@@ -12088,7 +12410,7 @@
       <c r="M131" s="20">
         <v>0.326</v>
       </c>
-      <c r="N131" s="24">
+      <c r="N131" s="28">
         <v>0.5</v>
       </c>
     </row>
@@ -12132,7 +12454,7 @@
       <c r="M132" s="20">
         <v>0.311</v>
       </c>
-      <c r="N132" s="24">
+      <c r="N132" s="28">
         <v>0.49</v>
       </c>
     </row>
@@ -12176,7 +12498,7 @@
       <c r="M133" s="20">
         <v>0.5</v>
       </c>
-      <c r="N133" s="24">
+      <c r="N133" s="28">
         <v>0.692</v>
       </c>
     </row>
@@ -12220,7 +12542,7 @@
       <c r="M134" s="20">
         <v>0.511</v>
       </c>
-      <c r="N134" s="24">
+      <c r="N134" s="28">
         <v>0.693</v>
       </c>
     </row>
@@ -12264,7 +12586,7 @@
       <c r="M135" s="20">
         <v>0.502</v>
       </c>
-      <c r="N135" s="24">
+      <c r="N135" s="28">
         <v>0.692</v>
       </c>
     </row>
@@ -12351,16 +12673,16 @@
       <c r="M1" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="P1" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="27" t="s">
         <v>122</v>
       </c>
     </row>
@@ -12404,16 +12726,16 @@
       <c r="M2" s="20">
         <v>0.92613</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="28">
         <v>0.74514</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="28">
         <v>0.88493</v>
       </c>
-      <c r="P2" s="24">
+      <c r="P2" s="28">
         <v>0.28439</v>
       </c>
-      <c r="Q2" s="24">
+      <c r="Q2" s="28">
         <v>0.79816</v>
       </c>
     </row>
@@ -12457,16 +12779,16 @@
       <c r="M3" s="20">
         <v>0.8896</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="28">
         <v>0.7498</v>
       </c>
-      <c r="O3" s="24">
+      <c r="O3" s="28">
         <v>0.887</v>
       </c>
-      <c r="P3" s="24">
+      <c r="P3" s="28">
         <v>0.2491</v>
       </c>
-      <c r="Q3" s="24">
+      <c r="Q3" s="28">
         <v>0.605</v>
       </c>
     </row>
@@ -12510,16 +12832,16 @@
       <c r="M4" s="20">
         <v>0.8924</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="28">
         <v>0.7655</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="28">
         <v>0.89</v>
       </c>
-      <c r="P4" s="24">
+      <c r="P4" s="28">
         <v>0.2493</v>
       </c>
-      <c r="Q4" s="24">
+      <c r="Q4" s="28">
         <v>0.6487</v>
       </c>
     </row>
@@ -12563,16 +12885,16 @@
       <c r="M5" s="20">
         <v>0.9007</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="28">
         <v>0.8002</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5" s="28">
         <v>0.909</v>
       </c>
-      <c r="P5" s="24">
+      <c r="P5" s="28">
         <v>0.2503</v>
       </c>
-      <c r="Q5" s="24">
+      <c r="Q5" s="28">
         <v>0.8137</v>
       </c>
     </row>
@@ -12616,16 +12938,16 @@
       <c r="M6" s="20">
         <v>0.9126</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="28">
         <v>0.8328</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6" s="28">
         <v>0.9093</v>
       </c>
-      <c r="P6" s="24">
+      <c r="P6" s="28">
         <v>0.2545</v>
       </c>
-      <c r="Q6" s="24">
+      <c r="Q6" s="28">
         <v>0.8176</v>
       </c>
     </row>
@@ -13033,7 +13355,7 @@
       <c r="M1" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="27" t="s">
         <v>138</v>
       </c>
     </row>
@@ -13077,7 +13399,7 @@
       <c r="M2" s="20">
         <v>0.541</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="28">
         <v>0.844</v>
       </c>
     </row>
@@ -13121,7 +13443,7 @@
       <c r="M3" s="20">
         <v>0.574</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="28">
         <v>0.85</v>
       </c>
     </row>
@@ -13165,7 +13487,7 @@
       <c r="M4" s="20">
         <v>0.556</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="28">
         <v>0.85</v>
       </c>
     </row>
@@ -13209,7 +13531,7 @@
       <c r="M5" s="20">
         <v>0.477</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="28">
         <v>0.828</v>
       </c>
     </row>
@@ -13253,7 +13575,7 @@
       <c r="M6" s="20">
         <v>0.666</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="28">
         <v>0.886</v>
       </c>
     </row>
@@ -13297,7 +13619,7 @@
       <c r="M7" s="20">
         <v>0.533</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="28">
         <v>0.851</v>
       </c>
     </row>
@@ -13341,7 +13663,7 @@
       <c r="M8" s="20">
         <v>0.557</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8" s="28">
         <v>0.851</v>
       </c>
     </row>
@@ -13385,7 +13707,7 @@
       <c r="M9" s="20">
         <v>0.572</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="28">
         <v>0.845</v>
       </c>
     </row>
@@ -13429,7 +13751,7 @@
       <c r="M10" s="20">
         <v>0.572</v>
       </c>
-      <c r="N10" s="24">
+      <c r="N10" s="28">
         <v>0.852</v>
       </c>
     </row>

</xml_diff>